<commit_message>
added sales and mbq trigger doc
</commit_message>
<xml_diff>
--- a/Ordering System/3dep calc/order home/gg.xlsx
+++ b/Ordering System/3dep calc/order home/gg.xlsx
@@ -21,6 +21,7 @@
     <sheet name="sales" sheetId="3" r:id="rId12"/>
     <sheet name="mbq" sheetId="2" r:id="rId13"/>
     <sheet name="stock" sheetId="4" r:id="rId14"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="109">
   <si>
     <t>MANGO MALDA</t>
   </si>
@@ -1647,9 +1648,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D5" sqref="D5:D30"/>
+      <selection pane="topRight" activeCell="A5" sqref="A5:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4094,7 +4095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2:N27"/>
     </sheetView>
   </sheetViews>
@@ -4816,6 +4817,44 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A5:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>